<commit_message>
distribute functions per files - started
</commit_message>
<xml_diff>
--- a/output/concentrations/ds.5p/xlsx/big_ser_test_res.xlsx
+++ b/output/concentrations/ds.5p/xlsx/big_ser_test_res.xlsx
@@ -1100,52 +1100,52 @@
     </row>
     <row r="2" spans="1:17">
       <c r="A2">
-        <v>5.471930600758339e-08</v>
+        <v>5.471930600758359e-08</v>
       </c>
       <c r="B2">
-        <v>4.356481401231441e-06</v>
+        <v>4.356481401231417e-06</v>
       </c>
       <c r="C2">
         <v>8.259517860200998e-05</v>
       </c>
       <c r="D2">
-        <v>1.081213216203394e-09</v>
+        <v>1.081213216202099e-09</v>
       </c>
       <c r="E2">
-        <v>7.452066594657265e-20</v>
+        <v>7.452066594656948e-20</v>
       </c>
       <c r="F2">
-        <v>0.07199070804429436</v>
+        <v>0.07199070804429411</v>
       </c>
       <c r="G2">
         <v>0.01680416842176199</v>
       </c>
       <c r="H2">
-        <v>6.661278729788259e-08</v>
+        <v>6.661278729788306e-08</v>
       </c>
       <c r="I2">
-        <v>1.384164767812207e-07</v>
+        <v>1.384164767810545e-07</v>
       </c>
       <c r="J2">
-        <v>2.808434087000289e-07</v>
+        <v>2.808434086996897e-07</v>
       </c>
       <c r="K2">
-        <v>2.879574846677609e-10</v>
+        <v>2.879574846674172e-10</v>
       </c>
       <c r="L2">
-        <v>2.425187923593632e-11</v>
+        <v>2.425187923590737e-11</v>
       </c>
       <c r="M2">
-        <v>2.217025891094558e-10</v>
+        <v>2.217025891091896e-10</v>
       </c>
       <c r="N2">
         <v>5.71419026054514e-10</v>
       </c>
       <c r="O2">
-        <v>9.502124992473862e-06</v>
+        <v>9.50212499246245e-06</v>
       </c>
       <c r="P2">
-        <v>2.547933406246887e-20</v>
+        <v>2.547933406243737e-20</v>
       </c>
       <c r="Q2" t="s">
         <v>8</v>
@@ -1162,7 +1162,7 @@
         <v>6.478803798340729e-05</v>
       </c>
       <c r="D3">
-        <v>3.403799932182848e-09</v>
+        <v>3.403799932182812e-09</v>
       </c>
       <c r="E3">
         <v>4.816083294337537e-20</v>
@@ -1177,28 +1177,28 @@
         <v>3.611237190463088e-08</v>
       </c>
       <c r="I3">
-        <v>4.588398451095249e-07</v>
+        <v>4.588398451095184e-07</v>
       </c>
       <c r="J3">
-        <v>9.802982417111789e-07</v>
+        <v>9.802982417111649e-07</v>
       </c>
       <c r="K3">
         <v>6.849211576790937e-10</v>
       </c>
       <c r="L3">
-        <v>4.358300176601331e-11</v>
+        <v>4.358300176601269e-11</v>
       </c>
       <c r="M3">
-        <v>9.7271265864213e-10</v>
+        <v>9.727126586421196e-10</v>
       </c>
       <c r="N3">
         <v>4.48223712219935e-10</v>
       </c>
       <c r="O3">
-        <v>1.840575689658404e-05</v>
+        <v>1.840575689658391e-05</v>
       </c>
       <c r="P3">
-        <v>5.183916705714027e-20</v>
+        <v>5.183916705713953e-20</v>
       </c>
       <c r="Q3" t="s">
         <v>8</v>
@@ -1209,13 +1209,13 @@
         <v>5.472287028230582e-08</v>
       </c>
       <c r="B4">
-        <v>3.99291961879964e-06</v>
+        <v>3.992919618799648e-06</v>
       </c>
       <c r="C4">
         <v>4.810700239698601e-05</v>
       </c>
       <c r="D4">
-        <v>8.971140220376932e-09</v>
+        <v>8.971140220376964e-09</v>
       </c>
       <c r="E4">
         <v>2.60625463599898e-20</v>
@@ -1224,13 +1224,13 @@
         <v>0.06598715982023311</v>
       </c>
       <c r="G4">
-        <v>0.01540381537647632</v>
+        <v>0.01540381537647643</v>
       </c>
       <c r="H4">
         <v>6.106567658839566e-08</v>
       </c>
       <c r="I4">
-        <v>1.052705958060878e-06</v>
+        <v>1.052705958060885e-06</v>
       </c>
       <c r="J4">
         <v>1.95779185358042e-06</v>
@@ -1239,10 +1239,10 @@
         <v>2.190160537476797e-09</v>
       </c>
       <c r="L4">
-        <v>1.690846777941723e-10</v>
+        <v>1.690846777941747e-10</v>
       </c>
       <c r="M4">
-        <v>1.839410986935779e-09</v>
+        <v>1.839410986935786e-09</v>
       </c>
       <c r="N4">
         <v>3.328191417630642e-10</v>
@@ -1259,52 +1259,52 @@
     </row>
     <row r="5" spans="1:17">
       <c r="A5">
-        <v>5.472794061560738e-08</v>
+        <v>5.472794061560855e-08</v>
       </c>
       <c r="B5">
-        <v>3.810716080097701e-06</v>
+        <v>3.810716080097586e-06</v>
       </c>
       <c r="C5">
-        <v>3.520489829357488e-05</v>
+        <v>3.520489829421788e-05</v>
       </c>
       <c r="D5">
-        <v>2.079209581070944e-08</v>
+        <v>2.079209580854643e-08</v>
       </c>
       <c r="E5">
-        <v>1.320125396748132e-20</v>
+        <v>1.320125396819626e-20</v>
       </c>
       <c r="F5">
-        <v>0.06298189140324958</v>
+        <v>0.06298189140324913</v>
       </c>
       <c r="G5">
-        <v>0.01470363810072552</v>
+        <v>0.01470363810072573</v>
       </c>
       <c r="H5">
-        <v>5.829534959538155e-08</v>
+        <v>5.829534959538362e-08</v>
       </c>
       <c r="I5">
-        <v>2.328702269840826e-06</v>
+        <v>2.328702269598553e-06</v>
       </c>
       <c r="J5">
-        <v>4.133611580623404e-06</v>
+        <v>4.133611580193353e-06</v>
       </c>
       <c r="K5">
-        <v>4.845326785254299e-09</v>
+        <v>4.84532678475034e-09</v>
       </c>
       <c r="L5">
-        <v>3.570654895631718e-10</v>
+        <v>3.570654895260388e-10</v>
       </c>
       <c r="M5">
-        <v>4.262743114543116e-09</v>
+        <v>4.262743114099569e-09</v>
       </c>
       <c r="N5">
-        <v>2.435583896754631e-10</v>
+        <v>2.435583896799107e-10</v>
       </c>
       <c r="O5">
-        <v>3.319742938003905e-05</v>
+        <v>3.319742937779818e-05</v>
       </c>
       <c r="P5">
-        <v>8.679874660303066e-20</v>
+        <v>8.679874659870236e-20</v>
       </c>
       <c r="Q5" t="s">
         <v>9</v>
@@ -1312,19 +1312,19 @@
     </row>
     <row r="6" spans="1:17">
       <c r="A6">
-        <v>5.473651091467158e-08</v>
+        <v>5.473651091467139e-08</v>
       </c>
       <c r="B6">
-        <v>3.628115830173309e-06</v>
+        <v>3.628115830173329e-06</v>
       </c>
       <c r="C6">
-        <v>2.643535036864405e-05</v>
+        <v>2.643535036871176e-05</v>
       </c>
       <c r="D6">
-        <v>4.174576686516881e-08</v>
+        <v>4.174576686484816e-08</v>
       </c>
       <c r="E6">
-        <v>7.041673031468728e-21</v>
+        <v>7.041673031512358e-21</v>
       </c>
       <c r="F6">
         <v>0.05997334253839248</v>
@@ -1336,28 +1336,28 @@
         <v>5.552805679012911e-08</v>
       </c>
       <c r="I6">
-        <v>4.452159326695709e-06</v>
+        <v>4.452159326661512e-06</v>
       </c>
       <c r="J6">
-        <v>7.525388963257135e-06</v>
+        <v>7.525388963199386e-06</v>
       </c>
       <c r="K6">
-        <v>9.265050874300005e-09</v>
+        <v>9.265050874228841e-09</v>
       </c>
       <c r="L6">
-        <v>6.502542109907156e-10</v>
+        <v>6.502542109857164e-10</v>
       </c>
       <c r="M6">
-        <v>8.557271924899375e-09</v>
+        <v>8.557271924833677e-09</v>
       </c>
       <c r="N6">
-        <v>1.828879411212124e-10</v>
+        <v>1.828879411216808e-10</v>
       </c>
       <c r="O6">
-        <v>3.758223337444669e-05</v>
+        <v>3.758223337435055e-05</v>
       </c>
       <c r="P6">
-        <v>9.295832697271403e-20</v>
+        <v>9.295832697257532e-20</v>
       </c>
       <c r="Q6" t="s">
         <v>10</v>
@@ -1365,46 +1365,46 @@
     </row>
     <row r="7" spans="1:17">
       <c r="A7">
-        <v>5.474828124361408e-08</v>
+        <v>5.474828124361447e-08</v>
       </c>
       <c r="B7">
-        <v>3.445226938358781e-06</v>
+        <v>3.445226938358738e-06</v>
       </c>
       <c r="C7">
-        <v>2.08363248078989e-05</v>
+        <v>2.083632480789901e-05</v>
       </c>
       <c r="D7">
-        <v>7.22009754521899e-08</v>
+        <v>7.220097545218914e-08</v>
       </c>
       <c r="E7">
-        <v>4.196047184234246e-21</v>
+        <v>4.196047184234306e-21</v>
       </c>
       <c r="F7">
-        <v>0.05696240586654119</v>
+        <v>0.05696240586654078</v>
       </c>
       <c r="G7">
         <v>0.01330328249663068</v>
       </c>
       <c r="H7">
-        <v>5.276297841589168e-08</v>
+        <v>5.276297841589205e-08</v>
       </c>
       <c r="I7">
-        <v>7.313603115111066e-06</v>
+        <v>7.313603115110911e-06</v>
       </c>
       <c r="J7">
-        <v>1.174139538222179e-05</v>
+        <v>1.174139538222146e-05</v>
       </c>
       <c r="K7">
-        <v>1.522305717455565e-08</v>
+        <v>1.522305717455544e-08</v>
       </c>
       <c r="L7">
-        <v>1.014987495810209e-09</v>
+        <v>1.014987495810195e-09</v>
       </c>
       <c r="M7">
-        <v>1.479696257778123e-08</v>
+        <v>1.479696257778097e-08</v>
       </c>
       <c r="N7">
-        <v>1.441521482223101e-10</v>
+        <v>1.441521482223106e-10</v>
       </c>
       <c r="O7">
         <v>4.038176551997847e-05</v>
@@ -1418,52 +1418,52 @@
     </row>
     <row r="8" spans="1:17">
       <c r="A8">
-        <v>5.47626832629991e-08</v>
+        <v>5.476268326299871e-08</v>
       </c>
       <c r="B8">
-        <v>3.262181506338455e-06</v>
+        <v>3.262181506338478e-06</v>
       </c>
       <c r="C8">
-        <v>1.71176203728305e-05</v>
+        <v>1.711762037266456e-05</v>
       </c>
       <c r="D8">
-        <v>1.119048096652854e-07</v>
+        <v>1.119048096678588e-07</v>
       </c>
       <c r="E8">
-        <v>2.748203447666309e-21</v>
+        <v>2.748203447606947e-21</v>
       </c>
       <c r="F8">
         <v>0.05395017290376282</v>
       </c>
       <c r="G8">
-        <v>0.01260310517217839</v>
+        <v>0.01260310517217821</v>
       </c>
       <c r="H8">
-        <v>4.999911070942407e-08</v>
+        <v>4.999911070942336e-08</v>
       </c>
       <c r="I8">
-        <v>1.073597752781412e-05</v>
+        <v>1.073597752806097e-05</v>
       </c>
       <c r="J8">
-        <v>1.632429500948693e-05</v>
+        <v>1.632429500986251e-05</v>
       </c>
       <c r="K8">
-        <v>2.235251079684457e-08</v>
+        <v>2.235251079735837e-08</v>
       </c>
       <c r="L8">
-        <v>1.411899790425707e-09</v>
+        <v>1.411899790458131e-09</v>
       </c>
       <c r="M8">
-        <v>2.292788703698051e-08</v>
+        <v>2.292788703750794e-08</v>
       </c>
       <c r="N8">
-        <v>1.184249992235709e-10</v>
+        <v>1.184249992224227e-10</v>
       </c>
       <c r="O8">
-        <v>4.224113062521071e-05</v>
+        <v>4.224113062536318e-05</v>
       </c>
       <c r="P8">
-        <v>9.725179657886384e-20</v>
+        <v>9.725179657899928e-20</v>
       </c>
       <c r="Q8" t="s">
         <v>10</v>
@@ -1474,46 +1474,46 @@
         <v>5.477943844784297e-08</v>
       </c>
       <c r="B9">
-        <v>3.079063770054671e-06</v>
+        <v>3.079063770054666e-06</v>
       </c>
       <c r="C9">
-        <v>1.447752824728147e-05</v>
+        <v>1.447752824728188e-05</v>
       </c>
       <c r="D9">
-        <v>1.613284092044167e-07</v>
+        <v>1.613284092044056e-07</v>
       </c>
       <c r="E9">
-        <v>1.922466080266764e-21</v>
+        <v>1.922466080266887e-21</v>
       </c>
       <c r="F9">
         <v>0.05093733972013908</v>
       </c>
       <c r="G9">
-        <v>0.01190292879117023</v>
+        <v>0.01190292879117014</v>
       </c>
       <c r="H9">
         <v>4.723581482237041e-08</v>
       </c>
       <c r="I9">
-        <v>1.461325998649189e-05</v>
+        <v>1.461325998649096e-05</v>
       </c>
       <c r="J9">
-        <v>2.097893176913461e-05</v>
+        <v>2.097893176913312e-05</v>
       </c>
       <c r="K9">
-        <v>3.043439597862091e-08</v>
+        <v>3.043439597861853e-08</v>
       </c>
       <c r="L9">
-        <v>1.815593094792928e-09</v>
+        <v>1.815593094792773e-09</v>
       </c>
       <c r="M9">
-        <v>3.304405036989968e-08</v>
+        <v>3.304405036989733e-08</v>
       </c>
       <c r="N9">
-        <v>1.001600242382305e-10</v>
+        <v>1.001600242382333e-10</v>
       </c>
       <c r="O9">
-        <v>4.356118579638462e-05</v>
+        <v>4.356118579638399e-05</v>
       </c>
       <c r="P9">
         <v>9.807753391976785e-20</v>
@@ -1527,49 +1527,49 @@
         <v>5.479856550316257e-08</v>
       </c>
       <c r="B10">
-        <v>2.895919008037259e-06</v>
+        <v>2.895919008037269e-06</v>
       </c>
       <c r="C10">
-        <v>1.248606345056467e-05</v>
+        <v>1.248606345056469e-05</v>
       </c>
       <c r="D10">
-        <v>2.218524029222349e-07</v>
+        <v>2.218524029222345e-07</v>
       </c>
       <c r="E10">
-        <v>1.405365041953481e-21</v>
+        <v>1.405365041953491e-21</v>
       </c>
       <c r="F10">
-        <v>0.04792428049144485</v>
+        <v>0.04792428049144502</v>
       </c>
       <c r="G10">
-        <v>0.01120275378640446</v>
+        <v>0.01120275378640454</v>
       </c>
       <c r="H10">
-        <v>4.447274957576346e-08</v>
+        <v>4.447274957576378e-08</v>
       </c>
       <c r="I10">
         <v>1.890687436451033e-05</v>
       </c>
       <c r="J10">
-        <v>2.553732124423323e-05</v>
+        <v>2.55373212442336e-05</v>
       </c>
       <c r="K10">
         <v>3.939026732318205e-08</v>
       </c>
       <c r="L10">
-        <v>2.211636350226684e-09</v>
+        <v>2.211636350226715e-09</v>
       </c>
       <c r="M10">
-        <v>4.542500117007921e-08</v>
+        <v>4.542500117007906e-08</v>
       </c>
       <c r="N10">
-        <v>8.638245399959584e-11</v>
+        <v>8.638245399959615e-11</v>
       </c>
       <c r="O10">
-        <v>4.455692508349039e-05</v>
+        <v>4.45569250834907e-05</v>
       </c>
       <c r="P10">
-        <v>9.85946349580465e-20</v>
+        <v>9.85946349580479e-20</v>
       </c>
       <c r="Q10" t="s">
         <v>11</v>
@@ -1580,19 +1580,19 @@
         <v>5.472288754799019e-08</v>
       </c>
       <c r="B11">
-        <v>2.722439150827053e-06</v>
+        <v>2.722439150827058e-06</v>
       </c>
       <c r="C11">
-        <v>4.295780970943569e-05</v>
+        <v>4.29578097093822e-05</v>
       </c>
       <c r="D11">
-        <v>1.23337098223445e-08</v>
+        <v>1.233370982238411e-08</v>
       </c>
       <c r="E11">
-        <v>1.734601305261121e-05</v>
+        <v>1.734601305255485e-05</v>
       </c>
       <c r="F11">
-        <v>0.04499115964694601</v>
+        <v>0.04499115964694617</v>
       </c>
       <c r="G11">
         <v>0.01050258470471664</v>
@@ -1601,28 +1601,28 @@
         <v>4.16356355615795e-08</v>
       </c>
       <c r="I11">
-        <v>9.867813066528112e-07</v>
+        <v>9.867813066559874e-07</v>
       </c>
       <c r="J11">
-        <v>1.251261554704523e-06</v>
+        <v>1.25126155470856e-06</v>
       </c>
       <c r="K11">
-        <v>2.053004585266921e-09</v>
+        <v>2.053004585273515e-09</v>
       </c>
       <c r="L11">
-        <v>1.080652623676399e-10</v>
+        <v>1.08065262367987e-10</v>
       </c>
       <c r="M11">
-        <v>2.528859614460191e-09</v>
+        <v>2.528859614468313e-09</v>
       </c>
       <c r="N11">
-        <v>2.971954319982975e-10</v>
+        <v>2.971954319979268e-10</v>
       </c>
       <c r="O11">
-        <v>2.932094654821348e-05</v>
+        <v>2.932094654823452e-05</v>
       </c>
       <c r="P11">
-        <v>6.765398695385759e-05</v>
+        <v>6.765398695385519e-05</v>
       </c>
       <c r="Q11" t="s">
         <v>11</v>
@@ -1636,13 +1636,13 @@
         <v>2.722785342797715e-06</v>
       </c>
       <c r="C12">
-        <v>7.104717707840947e-05</v>
+        <v>7.104717707827014e-05</v>
       </c>
       <c r="D12">
-        <v>2.226178028206273e-09</v>
+        <v>2.22617802822111e-09</v>
       </c>
       <c r="E12">
-        <v>4.988323497784697e-05</v>
+        <v>4.988323497739195e-05</v>
       </c>
       <c r="F12">
         <v>0.04499402045303055</v>
@@ -1654,28 +1654,28 @@
         <v>4.163298941500366e-08</v>
       </c>
       <c r="I12">
-        <v>1.781208231482807e-07</v>
+        <v>1.781208231494679e-07</v>
       </c>
       <c r="J12">
-        <v>2.258756913643002e-07</v>
+        <v>2.258756913658024e-07</v>
       </c>
       <c r="K12">
-        <v>3.705579121948515e-10</v>
+        <v>3.705579121973265e-10</v>
       </c>
       <c r="L12">
-        <v>1.950528451475127e-11</v>
+        <v>1.950528451488155e-11</v>
       </c>
       <c r="M12">
-        <v>4.564765739082761e-10</v>
+        <v>4.564765739113185e-10</v>
       </c>
       <c r="N12">
-        <v>4.915263749920553e-10</v>
+        <v>4.915263749910913e-10</v>
       </c>
       <c r="O12">
-        <v>1.447616570023402e-05</v>
+        <v>1.447616570027372e-05</v>
       </c>
       <c r="P12">
-        <v>3.51167650716732e-05</v>
+        <v>3.511676507158699e-05</v>
       </c>
       <c r="Q12" t="s">
         <v>11</v>
@@ -1728,7 +1728,7 @@
         <v>0.0005624203012347578</v>
       </c>
       <c r="E2">
-        <v>18.70497045762571</v>
+        <v>18.70497045760325</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1748,7 +1748,7 @@
         <v>0.0004411650710826132</v>
       </c>
       <c r="E3">
-        <v>36.23180491453552</v>
+        <v>36.23180491453526</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -1779,16 +1779,16 @@
         <v>26</v>
       </c>
       <c r="B5">
-        <v>4.453396906014182</v>
+        <v>4.45339690600625</v>
       </c>
       <c r="C5">
-        <v>34.65049044643197</v>
+        <v>34.65049044706485</v>
       </c>
       <c r="D5">
-        <v>0.0002397228244837235</v>
+        <v>0.0002397228244881011</v>
       </c>
       <c r="E5">
-        <v>65.34927043314774</v>
+        <v>65.34927042873656</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -1799,16 +1799,16 @@
         <v>27</v>
       </c>
       <c r="B6">
-        <v>4.57781492917185</v>
+        <v>4.577814929170737</v>
       </c>
       <c r="C6">
-        <v>26.01904563842918</v>
+        <v>26.01904563849583</v>
       </c>
       <c r="D6">
-        <v>0.0001800078160641854</v>
+        <v>0.0001800078160646465</v>
       </c>
       <c r="E6">
-        <v>73.98077435914702</v>
+        <v>73.98077435895777</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -1819,13 +1819,13 @@
         <v>28</v>
       </c>
       <c r="B7">
-        <v>4.681178881169332</v>
+        <v>4.68117888116933</v>
       </c>
       <c r="C7">
-        <v>20.50819370856191</v>
+        <v>20.50819370856202</v>
       </c>
       <c r="D7">
-        <v>0.00014188203565188</v>
+        <v>0.0001418820356518805</v>
       </c>
       <c r="E7">
         <v>79.49166440940645</v>
@@ -1839,16 +1839,16 @@
         <v>29</v>
       </c>
       <c r="B8">
-        <v>4.766556609447368</v>
+        <v>4.766556609451578</v>
       </c>
       <c r="C8">
-        <v>16.84805154806151</v>
+        <v>16.84805154789819</v>
       </c>
       <c r="D8">
-        <v>0.0001165600386058768</v>
+        <v>0.0001165600386047467</v>
       </c>
       <c r="E8">
-        <v>83.15183193939117</v>
+        <v>83.15183193969132</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -1859,16 +1859,16 @@
         <v>30</v>
       </c>
       <c r="B9">
-        <v>4.839305579036515</v>
+        <v>4.839305579036503</v>
       </c>
       <c r="C9">
-        <v>14.24953567645814</v>
+        <v>14.24953567645855</v>
       </c>
       <c r="D9">
-        <v>9.858270102188038e-05</v>
+        <v>9.858270102188319e-05</v>
       </c>
       <c r="E9">
-        <v>85.75036574091459</v>
+        <v>85.75036574091338</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
@@ -1882,13 +1882,13 @@
         <v>4.903574462440121</v>
       </c>
       <c r="C10">
-        <v>12.28943253008334</v>
+        <v>12.28943253008336</v>
       </c>
       <c r="D10">
-        <v>8.502210039330299e-05</v>
+        <v>8.502210039330329e-05</v>
       </c>
       <c r="E10">
-        <v>87.71048244781572</v>
+        <v>87.71048244781633</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -1899,16 +1899,16 @@
         <v>32</v>
       </c>
       <c r="B11">
-        <v>4.366957870124041</v>
+        <v>4.366957870124582</v>
       </c>
       <c r="C11">
-        <v>42.28130876912962</v>
+        <v>42.28130876907697</v>
       </c>
       <c r="D11">
-        <v>0.0002925151889747022</v>
+        <v>0.0002925151889743375</v>
       </c>
       <c r="E11">
-        <v>57.71839871695568</v>
+        <v>57.71839871699709</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -1919,16 +1919,16 @@
         <v>33</v>
       </c>
       <c r="B12">
-        <v>4.148453173241441</v>
+        <v>4.148453173242292</v>
       </c>
       <c r="C12">
-        <v>71.04717707840948</v>
+        <v>71.04717707827014</v>
       </c>
       <c r="D12">
-        <v>0.0004915263749920553</v>
+        <v>0.0004915263749910913</v>
       </c>
       <c r="E12">
-        <v>28.95233140046804</v>
+        <v>28.95233140054745</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>
@@ -1969,19 +1969,19 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2">
-        <v>3.191891195797325e-16</v>
+        <v>6.938893903907228e-17</v>
       </c>
       <c r="B2">
-        <v>3.191891195797325e-16</v>
+        <v>6.938893903907228e-17</v>
       </c>
       <c r="C2">
-        <v>5.983752447528967e-15</v>
+        <v>5.960929991798147e-15</v>
       </c>
       <c r="D2">
-        <v>3.124353870780951e-15</v>
+        <v>3.112434423147188e-15</v>
       </c>
       <c r="E2">
-        <v>9.04153090223108e-30</v>
+        <v>9.006852126169957e-30</v>
       </c>
       <c r="F2" t="s">
         <v>8</v>
@@ -1995,13 +1995,13 @@
         <v>-1.249000902703301e-16</v>
       </c>
       <c r="C3">
-        <v>2.875846262517801e-16</v>
+        <v>2.873271282358147e-16</v>
       </c>
       <c r="D3">
-        <v>1.550680157197393e-16</v>
+        <v>1.549155497892335e-16</v>
       </c>
       <c r="E3">
-        <v>5.156436684853776e-31</v>
+        <v>5.148973706319275e-31</v>
       </c>
       <c r="F3" t="s">
         <v>8</v>
@@ -2009,16 +2009,16 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4">
-        <v>-1.942890293094024e-16</v>
+        <v>2.775557561562891e-17</v>
       </c>
       <c r="B4">
-        <v>-6.938893903907228e-17</v>
+        <v>4.163336342344337e-17</v>
       </c>
       <c r="C4">
         <v>1.219727444046192e-18</v>
       </c>
       <c r="D4">
-        <v>6.844026213814747e-19</v>
+        <v>6.911788849595091e-19</v>
       </c>
       <c r="E4">
         <v>1.131483842327501e-33</v>
@@ -2029,19 +2029,19 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5">
-        <v>2.935152121352758e-13</v>
+        <v>2.92377233535035e-13</v>
       </c>
       <c r="B5">
-        <v>2.936123566499305e-13</v>
+        <v>2.922662112325725e-13</v>
       </c>
       <c r="C5">
-        <v>6.120426702341947e-13</v>
+        <v>6.082039169172382e-13</v>
       </c>
       <c r="D5">
-        <v>4.617034429473324e-13</v>
+        <v>4.587870881811451e-13</v>
       </c>
       <c r="E5">
-        <v>5.705119801905738e-28</v>
+        <v>5.668986226512874e-28</v>
       </c>
       <c r="F5" t="s">
         <v>9</v>
@@ -2049,19 +2049,19 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6">
-        <v>1.035282970462958e-14</v>
+        <v>1.020017403874363e-14</v>
       </c>
       <c r="B6">
-        <v>1.031119634120614e-14</v>
+        <v>1.015854067532018e-14</v>
       </c>
       <c r="C6">
-        <v>5.478541340205034e-15</v>
+        <v>5.353980063113606e-15</v>
       </c>
       <c r="D6">
-        <v>8.274983346115428e-15</v>
+        <v>8.086440588320198e-15</v>
       </c>
       <c r="E6">
-        <v>4.182758727344504e-30</v>
+        <v>4.087690010464689e-30</v>
       </c>
       <c r="F6" t="s">
         <v>10</v>
@@ -2069,19 +2069,19 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7">
-        <v>3.747002708109903e-16</v>
+        <v>-2.775557561562891e-17</v>
       </c>
       <c r="B7">
-        <v>3.747002708109903e-16</v>
+        <v>-2.775557561562891e-17</v>
       </c>
       <c r="C7">
-        <v>4.065758146820642e-18</v>
+        <v>4.174178364069192e-18</v>
       </c>
       <c r="D7">
-        <v>1.176359357146772e-17</v>
+        <v>1.127570259384925e-17</v>
       </c>
       <c r="E7">
-        <v>1.889818757929975e-33</v>
+        <v>1.950004068692076e-33</v>
       </c>
       <c r="F7" t="s">
         <v>10</v>
@@ -2089,19 +2089,19 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8">
-        <v>4.15487089178157e-13</v>
+        <v>4.161254674173165e-13</v>
       </c>
       <c r="B8">
-        <v>4.154315780269258e-13</v>
+        <v>4.16236489719779e-13</v>
       </c>
       <c r="C8">
-        <v>4.82511437489147e-14</v>
+        <v>4.83901520199545e-14</v>
       </c>
       <c r="D8">
-        <v>2.698013931408741e-13</v>
+        <v>2.705799451684088e-13</v>
       </c>
       <c r="E8">
-        <v>2.653015442935812e-29</v>
+        <v>2.660622866216141e-29</v>
       </c>
       <c r="F8" t="s">
         <v>10</v>
@@ -2109,19 +2109,19 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9">
-        <v>1.165734175856414e-15</v>
+        <v>9.992007221626409e-16</v>
       </c>
       <c r="B9">
-        <v>1.110223024625157e-15</v>
+        <v>1.02695629777827e-15</v>
       </c>
       <c r="C9">
-        <v>7.494547517306049e-17</v>
+        <v>7.410521848938423e-17</v>
       </c>
       <c r="D9">
-        <v>6.589374228552214e-16</v>
+        <v>6.558745517179498e-16</v>
       </c>
       <c r="E9">
-        <v>3.461859075036056e-32</v>
+        <v>3.473896137188477e-32</v>
       </c>
       <c r="F9" t="s">
         <v>10</v>
@@ -2129,19 +2129,19 @@
     </row>
     <row r="10" spans="1:6">
       <c r="A10">
-        <v>-1.387778780781446e-16</v>
+        <v>1.804112415015879e-16</v>
       </c>
       <c r="B10">
-        <v>-8.326672684688674e-17</v>
+        <v>1.734723475976807e-16</v>
       </c>
       <c r="C10">
-        <v>-5.421010862427522e-19</v>
+        <v>9.486769009248164e-20</v>
       </c>
       <c r="D10">
-        <v>-2.303929616531697e-19</v>
+        <v>4.472333961502706e-19</v>
       </c>
       <c r="E10">
-        <v>-1.203706215242022e-35</v>
+        <v>1.384262147528326e-33</v>
       </c>
       <c r="F10" t="s">
         <v>11</v>
@@ -2149,19 +2149,19 @@
     </row>
     <row r="11" spans="1:6">
       <c r="A11">
-        <v>1.804112415015879e-16</v>
+        <v>3.608224830031759e-16</v>
       </c>
       <c r="B11">
-        <v>2.220446049250313e-16</v>
+        <v>3.885780586188048e-16</v>
       </c>
       <c r="C11">
-        <v>1.294645814164941e-15</v>
+        <v>1.283234586299531e-15</v>
       </c>
       <c r="D11">
-        <v>2.712850018411761e-15</v>
+        <v>2.738762450334165e-15</v>
       </c>
       <c r="E11">
-        <v>6.468783841917514e-15</v>
+        <v>6.410033636695955e-15</v>
       </c>
       <c r="F11" t="s">
         <v>11</v>
@@ -2169,19 +2169,19 @@
     </row>
     <row r="12" spans="1:6">
       <c r="A12">
-        <v>4.302114220422482e-16</v>
+        <v>4.163336342344337e-16</v>
       </c>
       <c r="B12">
-        <v>3.400058012914542e-16</v>
+        <v>3.469446951953614e-16</v>
       </c>
       <c r="C12">
-        <v>5.252498739768963e-15</v>
+        <v>5.192583017211982e-15</v>
       </c>
       <c r="D12">
-        <v>4.21862387687752e-15</v>
+        <v>4.174828885372683e-15</v>
       </c>
       <c r="E12">
-        <v>4.952016173422752e-14</v>
+        <v>4.897894156224991e-14</v>
       </c>
       <c r="F12" t="s">
         <v>11</v>

</xml_diff>